<commit_message>
Abrir orden de análisis
</commit_message>
<xml_diff>
--- a/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-3.xlsx
+++ b/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-3.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="41">
   <si>
     <t xml:space="preserve">RESULTADO OBTENIDO </t>
   </si>
@@ -270,6 +270,30 @@
   </si>
   <si>
     <t>No mostrar atenciones</t>
+  </si>
+  <si>
+    <t>Crear muestra de análisis</t>
+  </si>
+  <si>
+    <t>Seleccionar atención e ingresar campo de comentario</t>
+  </si>
+  <si>
+    <t>Creación de resultado de atención</t>
+  </si>
+  <si>
+    <t>Abrir una orden de análisis</t>
+  </si>
+  <si>
+    <t>Seleccionar un resultado de atención y abrir la orden</t>
+  </si>
+  <si>
+    <t>Abrir orden sin seleccionar</t>
+  </si>
+  <si>
+    <t>No seleccionar atención e intentar agendar</t>
+  </si>
+  <si>
+    <t>Botón de abrir orden desactivado</t>
   </si>
 </sst>
 </file>
@@ -1115,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1315,12 +1339,12 @@
       <c r="K14" s="4"/>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="2:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" s="6">
         <v>3</v>
@@ -1328,9 +1352,15 @@
       <c r="E15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="F15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="I15" s="4" t="s">
         <v>14</v>
       </c>
@@ -1338,7 +1368,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="2:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1351,9 +1381,15 @@
       <c r="E16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="F16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="I16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1374,9 +1410,15 @@
       <c r="E17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="F17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="I17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1425,9 +1467,7 @@
       <c r="C20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="6">
-        <v>8</v>
-      </c>
+      <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
         <v>21</v>
       </c>
@@ -1448,9 +1488,7 @@
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="6">
-        <v>9</v>
-      </c>
+      <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
         <v>21</v>
       </c>
@@ -1471,9 +1509,7 @@
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="6">
-        <v>10</v>
-      </c>
+      <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
         <v>21</v>
       </c>
@@ -1492,9 +1528,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="6">
-        <v>11</v>
-      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="3"/>
       <c r="G23" s="2"/>
@@ -1513,9 +1547,7 @@
       <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="6">
-        <v>12</v>
-      </c>
+      <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
         <v>26</v>
       </c>
@@ -1536,9 +1568,7 @@
       <c r="C25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="6">
-        <v>13</v>
-      </c>
+      <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
         <v>26</v>
       </c>
@@ -1557,9 +1587,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="6">
-        <v>14</v>
-      </c>
+      <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="3"/>
       <c r="G26" s="2"/>
@@ -1578,9 +1606,7 @@
       <c r="C27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="6">
-        <v>15</v>
-      </c>
+      <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="3"/>
       <c r="G27" s="2"/>
@@ -1599,9 +1625,7 @@
       <c r="C28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="6">
-        <v>16</v>
-      </c>
+      <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="3"/>
       <c r="G28" s="2"/>
@@ -1618,9 +1642,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="6">
-        <v>17</v>
-      </c>
+      <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="3"/>
       <c r="G29" s="2"/>
@@ -1637,9 +1659,7 @@
         <v>20</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="6">
-        <v>18</v>
-      </c>
+      <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="3"/>
       <c r="G30" s="2"/>
@@ -1656,9 +1676,7 @@
         <v>20</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="6">
-        <v>19</v>
-      </c>
+      <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="3"/>
       <c r="G31" s="2"/>
@@ -1675,9 +1693,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="6">
-        <v>20</v>
-      </c>
+      <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="3"/>
       <c r="G32" s="2"/>

</xml_diff>

<commit_message>
Cerrar orden de análisis
</commit_message>
<xml_diff>
--- a/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-3.xlsx
+++ b/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-3.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t xml:space="preserve">RESULTADO OBTENIDO </t>
   </si>
@@ -290,10 +290,31 @@
     <t>Abrir orden sin seleccionar</t>
   </si>
   <si>
+    <t>Cerrar orden sin seleccionar</t>
+  </si>
+  <si>
     <t>No seleccionar atención e intentar agendar</t>
   </si>
   <si>
     <t>Botón de abrir orden desactivado</t>
+  </si>
+  <si>
+    <t>Cerrar orden de análisis sin archivo</t>
+  </si>
+  <si>
+    <t>No seleccionar atención e intentar cerrar la orden</t>
+  </si>
+  <si>
+    <t>Seleccionar un resultado de atención y no seleccionar archivo</t>
+  </si>
+  <si>
+    <t>Seleccionar un resultado de atención, seleccionar archivo y cerrar la orden</t>
+  </si>
+  <si>
+    <t>Desplegar mensaje de que falta archivo</t>
+  </si>
+  <si>
+    <t>Desplegar mensaje de que no se seleccionó archivo</t>
   </si>
 </sst>
 </file>
@@ -515,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -547,30 +568,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1137,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:M47"/>
+  <dimension ref="B5:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E23" sqref="D23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1158,116 +1155,116 @@
   <sheetData>
     <row r="5" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="20"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="22"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="22"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="23">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="17">
         <v>42703</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="24"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="20"/>
       <c r="M11" s="5"/>
     </row>
     <row r="12" spans="2:13" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B12" s="32"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1414,10 +1411,10 @@
         <v>38</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>14</v>
@@ -1426,16 +1423,28 @@
       <c r="K17" s="4"/>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="6">
+        <v>6</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="I18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1443,16 +1452,28 @@
       <c r="K18" s="4"/>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="6">
+        <v>7</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="I19" s="4" t="s">
         <v>14</v>
       </c>
@@ -1460,20 +1481,28 @@
       <c r="K19" s="4"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="2:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="6">
+        <v>8</v>
+      </c>
       <c r="E20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="F20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="I20" s="4" t="s">
         <v>14</v>
       </c>
@@ -1486,11 +1515,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="D21" s="6">
+        <v>9</v>
+      </c>
       <c r="E21" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="2"/>
@@ -1507,11 +1538,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="D22" s="6">
+        <v>10</v>
+      </c>
       <c r="E22" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="2"/>
@@ -1540,17 +1573,13 @@
       <c r="K23" s="4"/>
       <c r="L23" s="9"/>
     </row>
-    <row r="24" spans="2:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="3"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1565,13 +1594,9 @@
       <c r="B25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="3"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1598,397 +1623,6 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="9"/>
-    </row>
-    <row r="27" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="9"/>
-    </row>
-    <row r="28" spans="2:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="9"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="9"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="9"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="9"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="9"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="6">
-        <v>21</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="9"/>
-    </row>
-    <row r="34" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="6">
-        <v>22</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="9"/>
-    </row>
-    <row r="35" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="6">
-        <v>23</v>
-      </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="9"/>
-    </row>
-    <row r="36" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="6">
-        <v>24</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="9"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="6">
-        <v>25</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="9"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B38" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="6">
-        <v>26</v>
-      </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="9"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B39" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="6">
-        <v>27</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="9"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B40" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="6">
-        <v>28</v>
-      </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="9"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B41" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="6">
-        <v>29</v>
-      </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="9"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B42" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="6">
-        <v>30</v>
-      </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="9"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B43" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="6">
-        <v>31</v>
-      </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="9"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B44" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="6">
-        <v>32</v>
-      </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="9"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B45" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="6">
-        <v>33</v>
-      </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="9"/>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B46" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="6">
-        <v>34</v>
-      </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="9"/>
-    </row>
-    <row r="47" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="12">
-        <v>35</v>
-      </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>